<commit_message>
Fixed typo in lookup table
</commit_message>
<xml_diff>
--- a/Data/cellline_lookup.xlsx
+++ b/Data/cellline_lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phornauer/polybox/Sync/Protokolle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Promotion\Git\DeePhys\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91893396-B95B-6041-975E-16F0B8DAEB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EFB2A3-9FF1-4D86-867A-047F45660EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18400" yWindow="-22340" windowWidth="28040" windowHeight="16020" xr2:uid="{8B64A841-4996-5B47-B304-A4CAAD334927}"/>
+    <workbookView xWindow="-24150" yWindow="3915" windowWidth="19095" windowHeight="15150" xr2:uid="{8B64A841-4996-5B47-B304-A4CAAD334927}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>M05867_0,M05867_1,M05867_2</t>
   </si>
   <si>
-    <t>M05867_3,M05867_4M05867_5</t>
-  </si>
-  <si>
     <t>M04163_0,M04163_1,M04163_2</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>Chip_IDs</t>
+  </si>
+  <si>
+    <t>M05867_3,M05867_4,M05867_5</t>
   </si>
 </sst>
 </file>
@@ -249,7 +249,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -563,48 +563,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6635B43-8613-6540-96C9-FD7B17806B69}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="140.83203125" customWidth="1"/>
+    <col min="10" max="10" width="140.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>221207</v>
       </c>
@@ -636,7 +636,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>221207</v>
       </c>
@@ -668,7 +668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>221207</v>
       </c>
@@ -700,7 +700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>221208</v>
       </c>
@@ -729,10 +729,10 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>221207</v>
       </c>
@@ -764,7 +764,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>221207</v>
       </c>
@@ -796,7 +796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>221208</v>
       </c>
@@ -825,10 +825,10 @@
         <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>221208</v>
       </c>
@@ -857,10 +857,10 @@
         <v>20</v>
       </c>
       <c r="J9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>221208</v>
       </c>
@@ -889,10 +889,10 @@
         <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>221207</v>
       </c>
@@ -924,7 +924,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>221207</v>
       </c>
@@ -956,7 +956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>221208</v>
       </c>
@@ -985,10 +985,10 @@
         <v>20</v>
       </c>
       <c r="J13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>221207</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>221207</v>
       </c>
@@ -1049,10 +1049,10 @@
         <v>20</v>
       </c>
       <c r="J15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>221208</v>
       </c>
@@ -1081,10 +1081,10 @@
         <v>20</v>
       </c>
       <c r="J16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>221208</v>
       </c>
@@ -1113,10 +1113,10 @@
         <v>20</v>
       </c>
       <c r="J17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>221208</v>
       </c>
@@ -1145,10 +1145,10 @@
         <v>20</v>
       </c>
       <c r="J18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>221209</v>
       </c>
@@ -1177,10 +1177,10 @@
         <v>0</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>221209</v>
       </c>
@@ -1209,10 +1209,10 @@
         <v>0</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>221209</v>
       </c>
@@ -1241,10 +1241,10 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>221209</v>
       </c>
@@ -1273,10 +1273,10 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>221209</v>
       </c>
@@ -1305,10 +1305,10 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>221209</v>
       </c>
@@ -1337,10 +1337,10 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>221209</v>
       </c>
@@ -1369,10 +1369,10 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>221209</v>
       </c>
@@ -1401,10 +1401,10 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>221209</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>